<commit_message>
Added 3,3V and vias to Basisplatine, ...
</commit_message>
<xml_diff>
--- a/Basisplatine/Stueckliste.xlsx
+++ b/Basisplatine/Stueckliste.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Messbox\Basisplatine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klosskopf\Desktop\Arbeit\Messbox\Basisplatine\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D67DD2E-8A62-4C6E-AAD6-610F245C2174}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15750" windowHeight="20985"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="118">
   <si>
     <t>Bauteil</t>
   </si>
@@ -44,9 +51,6 @@
     <t>10uF 1206</t>
   </si>
   <si>
-    <t>NTS12120EMFST1G</t>
-  </si>
-  <si>
     <t>AP63205WU-7</t>
   </si>
   <si>
@@ -179,9 +183,6 @@
     <t>2k 0603</t>
   </si>
   <si>
-    <t>C11,C13,C12,C10,C6,C7,C8,C9,C31,C27,C28,C29,C30</t>
-  </si>
-  <si>
     <t>U1,U2,U3,U4,U5</t>
   </si>
   <si>
@@ -269,9 +270,6 @@
     <t>BLG2X10</t>
   </si>
   <si>
-    <t>U7,U9,U10,U11,U12</t>
-  </si>
-  <si>
     <t>R28,R26,R25,R24,R23,R22,R21,R20,R32,R37,R36,R35,R34,R33,R38,R39,R40</t>
   </si>
   <si>
@@ -291,13 +289,109 @@
   </si>
   <si>
     <t>1206DD106MAT2A</t>
+  </si>
+  <si>
+    <t>C11,C13,C12,C10,C6,C7,C8,C9,C31,C27,C28,C29,C30,C49,C50,C51,C52,C53,C54,C55,C56,C57,C58</t>
+  </si>
+  <si>
+    <t>Bestellnummer</t>
+  </si>
+  <si>
+    <t>1492267 - 62</t>
+  </si>
+  <si>
+    <t>1693283 - 62</t>
+  </si>
+  <si>
+    <t>556-ATMEGA88PB-AU</t>
+  </si>
+  <si>
+    <t>453-DIO5158XS8</t>
+  </si>
+  <si>
+    <t>595-TPS613222ADBVR</t>
+  </si>
+  <si>
+    <t>621-AP63205WU-7</t>
+  </si>
+  <si>
+    <t>449-LFXTAL002996BULK</t>
+  </si>
+  <si>
+    <t>863-NTF5P03T3G</t>
+  </si>
+  <si>
+    <t>771-BCW66HVL</t>
+  </si>
+  <si>
+    <t>652-SRN5040TA-4R7M</t>
+  </si>
+  <si>
+    <t>652-SRP1038C-2R2M</t>
+  </si>
+  <si>
+    <t>U9,U10,U11,U12</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>SBRT10U50SP5-13</t>
+  </si>
+  <si>
+    <t>621-SBRT10U50SP5-13</t>
+  </si>
+  <si>
+    <t>833-SK33-TP</t>
+  </si>
+  <si>
+    <t>SK33-TP</t>
+  </si>
+  <si>
+    <t>71-CRCW0603-4.99-E3</t>
+  </si>
+  <si>
+    <t>71-CRCW0603100RFKEAC</t>
+  </si>
+  <si>
+    <t>667-ERJ-3RBD1201V</t>
+  </si>
+  <si>
+    <t>754-RR0816P-202D</t>
+  </si>
+  <si>
+    <t>754-RR0816P-103D</t>
+  </si>
+  <si>
+    <t>754-RR0816P-823D</t>
+  </si>
+  <si>
+    <t>754-RR0816P-274D</t>
+  </si>
+  <si>
+    <t>806-KLDX-0202-AC</t>
+  </si>
+  <si>
+    <t>649-54601-908WPLF</t>
+  </si>
+  <si>
+    <t>80-C0603C121J5GAC</t>
+  </si>
+  <si>
+    <t>791-0603B104J500CT</t>
+  </si>
+  <si>
+    <t>581-1206DD106MAT2A</t>
+  </si>
+  <si>
+    <t>Euro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,16 +417,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -341,19 +447,36 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -361,7 +484,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -641,18 +766,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="79.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -666,70 +793,76 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="2">
+        <v>78</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>0.32</v>
       </c>
-      <c r="G2" s="2">
-        <f>F2*E2</f>
+      <c r="H2" s="2">
+        <f>G2*F2</f>
         <v>1.6</v>
       </c>
-      <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="2">
+        <v>67</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>20.16</v>
       </c>
-      <c r="G3" s="2">
-        <f>F3*E3</f>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H32" si="0">G3*F3</f>
         <v>20.16</v>
       </c>
-      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -738,392 +871,422 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="2">
+        <v>71</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>1.17</v>
       </c>
-      <c r="G5" s="2">
-        <f>F5*E5</f>
+      <c r="H5" s="2">
+        <f t="shared" si="0"/>
         <v>1.17</v>
       </c>
-      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="G6" s="2">
-        <f>F6*E6</f>
+      <c r="H6" s="2">
+        <f t="shared" si="0"/>
         <v>0.57999999999999996</v>
       </c>
-      <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>0.92</v>
       </c>
-      <c r="G7" s="2">
-        <f>F7*E7</f>
+      <c r="H7" s="2">
+        <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
-      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="2">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>1.31</v>
       </c>
-      <c r="G8" s="2">
-        <f>F8*E8</f>
+      <c r="H8" s="2">
+        <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="2">
+        <v>70</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>0.26</v>
       </c>
-      <c r="G9" s="2">
-        <f>F9*E9</f>
+      <c r="H9" s="2">
+        <f t="shared" si="0"/>
         <v>0.26</v>
       </c>
-      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G10" s="2">
-        <f>F10*E10</f>
+      <c r="H10" s="2">
+        <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
-      <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="2">
+        <v>62</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="2">
         <v>2</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>0.17</v>
       </c>
-      <c r="G11" s="2">
-        <f>F11*E11</f>
+      <c r="H11" s="2">
+        <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
-      <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="2">
         <v>1</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>0.34</v>
       </c>
-      <c r="G12" s="2">
-        <f>F12*E12</f>
+      <c r="H12" s="2">
+        <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
-      <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="2">
         <v>2</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>1.06</v>
       </c>
-      <c r="G13" s="2">
-        <f>F13*E13</f>
+      <c r="H13" s="2">
+        <f t="shared" si="0"/>
         <v>2.12</v>
       </c>
-      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="2">
-        <v>5</v>
+        <v>101</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F14" s="2">
-        <v>0.42</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2">
-        <f>F14*E14</f>
-        <v>2.1</v>
-      </c>
-      <c r="H14" s="2"/>
+        <v>0.61</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>99</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="2">
-        <v>1</v>
+        <v>17</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F15" s="2">
-        <v>0.1</v>
+        <v>4</v>
       </c>
       <c r="G15" s="2">
-        <f>F15*E15</f>
-        <v>0.1</v>
-      </c>
-      <c r="H15" s="2"/>
+        <v>0.35</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" s="2">
-        <v>17</v>
+        <v>64</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2">
         <v>0.1</v>
       </c>
-      <c r="G16" s="2">
-        <f>F16*E16</f>
-        <v>1.7000000000000002</v>
-      </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1</v>
+        <v>69</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F17" s="2">
-        <v>0.1</v>
+        <v>17</v>
       </c>
       <c r="G17" s="2">
-        <f>F17*E17</f>
-        <v>0.1</v>
-      </c>
-      <c r="H17" s="2"/>
+        <v>2.3E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <f>G17*F17</f>
+        <v>0.39100000000000001</v>
+      </c>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="2">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="2">
         <v>1</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>0.1</v>
       </c>
-      <c r="G18" s="2">
-        <f>F18*E18</f>
+      <c r="H18" s="2">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="2">
-        <v>13</v>
+        <v>77</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F19" s="2">
-        <v>0.12</v>
+        <v>1</v>
       </c>
       <c r="G19" s="2">
-        <f>F19*E19</f>
-        <v>1.56</v>
-      </c>
-      <c r="H19" s="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1131,185 +1294,223 @@
         <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="2">
-        <v>4</v>
+        <v>73</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F20" s="2">
-        <v>0.1</v>
+        <v>13</v>
       </c>
       <c r="G20" s="2">
-        <f>F20*E20</f>
-        <v>0.4</v>
-      </c>
-      <c r="H20" s="2"/>
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0529999999999999</v>
+      </c>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="2">
-        <v>1</v>
+        <v>72</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F21" s="2">
+        <v>4</v>
+      </c>
+      <c r="G21" s="2">
         <v>0.1</v>
       </c>
-      <c r="G21" s="2">
-        <f>F21*E21</f>
-        <v>0.1</v>
-      </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="2">
+        <v>75</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="2">
         <v>1</v>
       </c>
-      <c r="F22" s="2">
-        <v>0.44</v>
-      </c>
       <c r="G22" s="2">
-        <f>F22*E22</f>
-        <v>0.44</v>
-      </c>
-      <c r="H22" s="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.44</v>
+      </c>
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="D24" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="2">
         <v>5</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G24" s="2">
         <v>0.54</v>
       </c>
-      <c r="G23" s="2">
-        <f>F23*E23</f>
+      <c r="H24" s="2">
+        <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="2">
+        <v>59</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="2">
         <v>2</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>0.1</v>
       </c>
-      <c r="G25" s="2">
-        <f>F25*E25</f>
+      <c r="H25" s="2">
+        <f>G25*F25</f>
         <v>0.2</v>
       </c>
-      <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>51</v>
+        <v>86</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" s="2">
-        <v>13</v>
+        <v>58</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="F26" s="2">
-        <v>0.1</v>
+        <v>23</v>
       </c>
       <c r="G26" s="2">
-        <f>F26*E26</f>
-        <v>1.3</v>
-      </c>
-      <c r="H26" s="2"/>
+        <v>0.108</v>
+      </c>
+      <c r="H26" s="2">
+        <f>G26*F26</f>
+        <v>2.484</v>
+      </c>
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="2">
+        <v>85</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" s="2">
         <v>16</v>
       </c>
-      <c r="F27" s="2">
-        <v>0.23</v>
-      </c>
       <c r="G27" s="2">
-        <f>F27*E27</f>
-        <v>3.68</v>
-      </c>
-      <c r="H27" s="2"/>
+        <v>0.20899999999999999</v>
+      </c>
+      <c r="H27" s="2">
+        <f>G27*F27</f>
+        <v>3.3439999999999999</v>
+      </c>
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1318,84 +1519,85 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="F29" s="2">
         <v>1</v>
       </c>
-      <c r="F29" s="2">
+      <c r="G29" s="2">
         <v>0</v>
       </c>
-      <c r="G29" s="2">
-        <f>F29*E29</f>
+      <c r="H29" s="2">
+        <f>G29*F29</f>
         <v>0</v>
       </c>
-      <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E30" s="2">
+        <v>83</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="2">
         <v>2</v>
       </c>
-      <c r="F30" s="2">
+      <c r="G30" s="2">
         <v>0</v>
       </c>
-      <c r="G30" s="2">
-        <f>F30*E30</f>
+      <c r="H30" s="2">
+        <f>G30*F30</f>
         <v>0</v>
       </c>
-      <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="2">
+        <v>11</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F31" s="2">
         <v>1</v>
       </c>
-      <c r="F31" s="2">
+      <c r="G31" s="2">
         <v>0</v>
       </c>
-      <c r="G31" s="2">
-        <f>F31*E31</f>
+      <c r="H31" s="2">
+        <f>G31*F31</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="5">
-        <f>SUM(G2:G32)</f>
-        <v>43.560000000000009</v>
+    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G32" s="6">
+        <f>SUM(H2:H32)</f>
+        <v>42.50200000000001</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1408,5 +1610,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added cam for Basisplatine / Bestelldaten
</commit_message>
<xml_diff>
--- a/Basisplatine/Stueckliste.xlsx
+++ b/Basisplatine/Stueckliste.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klosskopf\Desktop\Arbeit\Messbox\Basisplatine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projekte\Messbox\Basisplatine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D67DD2E-8A62-4C6E-AAD6-610F245C2174}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
   <si>
     <t>Bauteil</t>
   </si>
@@ -300,12 +299,6 @@
     <t>1492267 - 62</t>
   </si>
   <si>
-    <t>1693283 - 62</t>
-  </si>
-  <si>
-    <t>556-ATMEGA88PB-AU</t>
-  </si>
-  <si>
     <t>453-DIO5158XS8</t>
   </si>
   <si>
@@ -384,14 +377,14 @@
     <t>581-1206DD106MAT2A</t>
   </si>
   <si>
-    <t>Euro</t>
+    <t>Mercateo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -423,6 +416,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -433,12 +432,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -446,37 +445,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -485,8 +458,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -766,11 +740,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="B20" sqref="B20:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +784,7 @@
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -838,67 +812,41 @@
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
-        <v>20.16</v>
-      </c>
-      <c r="H3" s="2">
-        <f t="shared" ref="H3:H32" si="0">G3*F3</f>
-        <v>20.16</v>
-      </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="H4" s="2"/>
+      <c r="D4" s="7">
+        <v>3272496006997</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>21.34</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4" si="0">G4*F4</f>
+        <v>21.34</v>
+      </c>
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1.17</v>
-      </c>
-      <c r="H5" s="2">
-        <f t="shared" si="0"/>
-        <v>1.17</v>
-      </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -908,7 +856,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>66</v>
@@ -920,13 +868,13 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="H6" s="2">
-        <f t="shared" si="0"/>
+        <f>G6*F6</f>
         <v>0.57999999999999996</v>
       </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -936,7 +884,7 @@
         <v>35</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>66</v>
@@ -948,13 +896,13 @@
         <v>0.92</v>
       </c>
       <c r="H7" s="2">
-        <f t="shared" si="0"/>
+        <f>G7*F7</f>
         <v>0.92</v>
       </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -964,7 +912,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>66</v>
@@ -976,13 +924,13 @@
         <v>1.31</v>
       </c>
       <c r="H8" s="2">
-        <f t="shared" si="0"/>
+        <f>G8*F8</f>
         <v>1.31</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -992,7 +940,7 @@
         <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>66</v>
@@ -1004,13 +952,13 @@
         <v>0.26</v>
       </c>
       <c r="H9" s="2">
-        <f t="shared" si="0"/>
+        <f>G9*F9</f>
         <v>0.26</v>
       </c>
       <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1020,7 +968,7 @@
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>66</v>
@@ -1032,13 +980,13 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="H10" s="2">
-        <f t="shared" si="0"/>
+        <f>G10*F10</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1048,7 +996,7 @@
         <v>62</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>66</v>
@@ -1060,13 +1008,13 @@
         <v>0.17</v>
       </c>
       <c r="H11" s="2">
-        <f t="shared" si="0"/>
+        <f>G11*F11</f>
         <v>0.34</v>
       </c>
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1076,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>66</v>
@@ -1088,13 +1036,13 @@
         <v>0.34</v>
       </c>
       <c r="H12" s="2">
-        <f t="shared" si="0"/>
+        <f>G12*F12</f>
         <v>0.34</v>
       </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1104,7 +1052,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>66</v>
@@ -1116,23 +1064,23 @@
         <v>1.06</v>
       </c>
       <c r="H13" s="2">
-        <f t="shared" si="0"/>
+        <f>G13*F13</f>
         <v>2.12</v>
       </c>
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>100</v>
+      <c r="A14" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>66</v>
@@ -1144,23 +1092,23 @@
         <v>0.61</v>
       </c>
       <c r="H14" s="2">
-        <f t="shared" si="0"/>
+        <f>G14*F14</f>
         <v>0.61</v>
       </c>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>99</v>
+      <c r="A15" s="6" t="s">
+        <v>97</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>66</v>
@@ -1172,13 +1120,13 @@
         <v>0.35</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="0"/>
+        <f>G15*F15</f>
         <v>1.4</v>
       </c>
       <c r="I15" s="2"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>31</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1188,7 +1136,7 @@
         <v>64</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>66</v>
@@ -1200,13 +1148,13 @@
         <v>0.1</v>
       </c>
       <c r="H16" s="2">
-        <f t="shared" si="0"/>
+        <f>G16*F16</f>
         <v>0.1</v>
       </c>
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>79</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1216,7 +1164,7 @@
         <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>66</v>
@@ -1234,7 +1182,7 @@
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1244,7 +1192,7 @@
         <v>60</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>66</v>
@@ -1256,13 +1204,13 @@
         <v>0.1</v>
       </c>
       <c r="H18" s="2">
-        <f t="shared" si="0"/>
+        <f>G18*F18</f>
         <v>0.1</v>
       </c>
       <c r="I18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1272,7 +1220,7 @@
         <v>77</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>66</v>
@@ -1284,13 +1232,13 @@
         <v>0.1</v>
       </c>
       <c r="H19" s="2">
-        <f t="shared" si="0"/>
+        <f>G19*F19</f>
         <v>0.1</v>
       </c>
       <c r="I19" s="2"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1300,7 +1248,7 @@
         <v>73</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>66</v>
@@ -1312,13 +1260,13 @@
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="H20" s="2">
-        <f t="shared" si="0"/>
+        <f>G20*F20</f>
         <v>1.0529999999999999</v>
       </c>
       <c r="I20" s="2"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1328,7 +1276,7 @@
         <v>72</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>66</v>
@@ -1340,13 +1288,13 @@
         <v>0.1</v>
       </c>
       <c r="H21" s="2">
-        <f t="shared" si="0"/>
+        <f>G21*F21</f>
         <v>0.4</v>
       </c>
       <c r="I21" s="2"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1356,7 +1304,7 @@
         <v>76</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>66</v>
@@ -1368,13 +1316,13 @@
         <v>0.1</v>
       </c>
       <c r="H22" s="2">
-        <f t="shared" si="0"/>
+        <f>G22*F22</f>
         <v>0.1</v>
       </c>
       <c r="I22" s="2"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1384,7 +1332,7 @@
         <v>57</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>66</v>
@@ -1396,13 +1344,13 @@
         <v>0.44</v>
       </c>
       <c r="H23" s="2">
-        <f t="shared" si="0"/>
+        <f>G23*F23</f>
         <v>0.44</v>
       </c>
       <c r="I23" s="2"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1412,7 +1360,7 @@
         <v>54</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>66</v>
@@ -1424,13 +1372,13 @@
         <v>0.54</v>
       </c>
       <c r="H24" s="2">
-        <f t="shared" si="0"/>
+        <f>G24*F24</f>
         <v>2.7</v>
       </c>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1440,7 +1388,7 @@
         <v>59</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>66</v>
@@ -1458,7 +1406,7 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="6" t="s">
         <v>86</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1468,7 +1416,7 @@
         <v>58</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>66</v>
@@ -1486,7 +1434,7 @@
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="6" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1496,7 +1444,7 @@
         <v>85</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>66</v>
@@ -1567,7 +1515,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>20</v>
       </c>
@@ -1591,13 +1539,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G32" s="6">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <f>G32*F32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="2">
         <f>SUM(H2:H32)</f>
-        <v>42.50200000000001</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>117</v>
+        <v>42.512000000000008</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>